<commit_message>
update "old" correct excel
....this means you can start editing this sheet again Sophia
</commit_message>
<xml_diff>
--- a/figures/fig_plans.xlsx
+++ b/figures/fig_plans.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Documents\HS_project\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB197EC6-678B-4431-888C-4BCC99E0CA17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB7D673-F0E7-4E1E-9571-11EF2A47F713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D0A47E1A-D9EC-4773-806B-C00D55A8027C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -492,13 +495,13 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="82" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.6640625" customWidth="1"/>
     <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>